<commit_message>
update before swine change to pigs
</commit_message>
<xml_diff>
--- a/fifth_pass/calc_tseries.xlsx
+++ b/fifth_pass/calc_tseries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jojos/Documents/GitHub/WAWex/first_pass/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jojos/Documents/GitHub/WAWex/fifth_pass/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A884F70C-628A-4A43-BF96-B87C207C2D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB2E366-A0B9-624A-A704-11E9B7C6C156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="17260" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,13 +100,13 @@
     <t>Sheep</t>
   </si>
   <si>
-    <t>Swine / pigs</t>
-  </si>
-  <si>
     <t>Turkeys</t>
   </si>
   <si>
     <t>NC_potential</t>
+  </si>
+  <si>
+    <t>Pigs</t>
   </si>
 </sst>
 </file>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A1040" workbookViewId="0">
+      <selection activeCell="E1071" sqref="E1071"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -481,7 +481,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -26703,7 +26703,7 @@
         <v>9</v>
       </c>
       <c r="B1010" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1010" s="2">
         <v>1961</v>
@@ -26729,7 +26729,7 @@
         <v>9</v>
       </c>
       <c r="B1011" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1011" s="2">
         <v>1962</v>
@@ -26755,7 +26755,7 @@
         <v>9</v>
       </c>
       <c r="B1012" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1012" s="2">
         <v>1963</v>
@@ -26781,7 +26781,7 @@
         <v>9</v>
       </c>
       <c r="B1013" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1013" s="2">
         <v>1964</v>
@@ -26807,7 +26807,7 @@
         <v>9</v>
       </c>
       <c r="B1014" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1014" s="2">
         <v>1965</v>
@@ -26833,7 +26833,7 @@
         <v>9</v>
       </c>
       <c r="B1015" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1015" s="2">
         <v>1966</v>
@@ -26859,7 +26859,7 @@
         <v>9</v>
       </c>
       <c r="B1016" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1016" s="2">
         <v>1967</v>
@@ -26885,7 +26885,7 @@
         <v>9</v>
       </c>
       <c r="B1017" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1017" s="2">
         <v>1968</v>
@@ -26911,7 +26911,7 @@
         <v>9</v>
       </c>
       <c r="B1018" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1018" s="2">
         <v>1969</v>
@@ -26937,7 +26937,7 @@
         <v>9</v>
       </c>
       <c r="B1019" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1019" s="2">
         <v>1970</v>
@@ -26963,7 +26963,7 @@
         <v>9</v>
       </c>
       <c r="B1020" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1020" s="2">
         <v>1971</v>
@@ -26989,7 +26989,7 @@
         <v>9</v>
       </c>
       <c r="B1021" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1021" s="2">
         <v>1972</v>
@@ -27015,7 +27015,7 @@
         <v>9</v>
       </c>
       <c r="B1022" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1022" s="2">
         <v>1973</v>
@@ -27041,7 +27041,7 @@
         <v>9</v>
       </c>
       <c r="B1023" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1023" s="2">
         <v>1974</v>
@@ -27067,7 +27067,7 @@
         <v>9</v>
       </c>
       <c r="B1024" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1024" s="2">
         <v>1975</v>
@@ -27093,7 +27093,7 @@
         <v>9</v>
       </c>
       <c r="B1025" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1025" s="2">
         <v>1976</v>
@@ -27119,7 +27119,7 @@
         <v>9</v>
       </c>
       <c r="B1026" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1026" s="2">
         <v>1977</v>
@@ -27145,7 +27145,7 @@
         <v>9</v>
       </c>
       <c r="B1027" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1027" s="2">
         <v>1978</v>
@@ -27171,7 +27171,7 @@
         <v>9</v>
       </c>
       <c r="B1028" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1028" s="2">
         <v>1979</v>
@@ -27197,7 +27197,7 @@
         <v>9</v>
       </c>
       <c r="B1029" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1029" s="2">
         <v>1980</v>
@@ -27223,7 +27223,7 @@
         <v>9</v>
       </c>
       <c r="B1030" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1030" s="2">
         <v>1981</v>
@@ -27249,7 +27249,7 @@
         <v>9</v>
       </c>
       <c r="B1031" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1031" s="2">
         <v>1982</v>
@@ -27275,7 +27275,7 @@
         <v>9</v>
       </c>
       <c r="B1032" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1032" s="2">
         <v>1983</v>
@@ -27301,7 +27301,7 @@
         <v>9</v>
       </c>
       <c r="B1033" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1033" s="2">
         <v>1984</v>
@@ -27327,7 +27327,7 @@
         <v>9</v>
       </c>
       <c r="B1034" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1034" s="2">
         <v>1985</v>
@@ -27353,7 +27353,7 @@
         <v>9</v>
       </c>
       <c r="B1035" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1035" s="2">
         <v>1986</v>
@@ -27379,7 +27379,7 @@
         <v>9</v>
       </c>
       <c r="B1036" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1036" s="2">
         <v>1987</v>
@@ -27405,7 +27405,7 @@
         <v>9</v>
       </c>
       <c r="B1037" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1037" s="2">
         <v>1988</v>
@@ -27431,7 +27431,7 @@
         <v>9</v>
       </c>
       <c r="B1038" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1038" s="2">
         <v>1989</v>
@@ -27457,7 +27457,7 @@
         <v>9</v>
       </c>
       <c r="B1039" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1039" s="2">
         <v>1990</v>
@@ -27483,7 +27483,7 @@
         <v>9</v>
       </c>
       <c r="B1040" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1040" s="2">
         <v>1991</v>
@@ -27509,7 +27509,7 @@
         <v>9</v>
       </c>
       <c r="B1041" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1041" s="2">
         <v>1992</v>
@@ -27535,7 +27535,7 @@
         <v>9</v>
       </c>
       <c r="B1042" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1042" s="2">
         <v>1993</v>
@@ -27561,7 +27561,7 @@
         <v>9</v>
       </c>
       <c r="B1043" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1043" s="2">
         <v>1994</v>
@@ -27587,7 +27587,7 @@
         <v>9</v>
       </c>
       <c r="B1044" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1044" s="2">
         <v>1995</v>
@@ -27613,7 +27613,7 @@
         <v>9</v>
       </c>
       <c r="B1045" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1045" s="2">
         <v>1996</v>
@@ -27639,7 +27639,7 @@
         <v>9</v>
       </c>
       <c r="B1046" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1046" s="2">
         <v>1997</v>
@@ -27665,7 +27665,7 @@
         <v>9</v>
       </c>
       <c r="B1047" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1047" s="2">
         <v>1998</v>
@@ -27691,7 +27691,7 @@
         <v>9</v>
       </c>
       <c r="B1048" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1048" s="2">
         <v>1999</v>
@@ -27717,7 +27717,7 @@
         <v>9</v>
       </c>
       <c r="B1049" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1049" s="2">
         <v>2000</v>
@@ -27743,7 +27743,7 @@
         <v>9</v>
       </c>
       <c r="B1050" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1050" s="2">
         <v>2001</v>
@@ -27769,7 +27769,7 @@
         <v>9</v>
       </c>
       <c r="B1051" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1051" s="2">
         <v>2002</v>
@@ -27795,7 +27795,7 @@
         <v>9</v>
       </c>
       <c r="B1052" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1052" s="2">
         <v>2003</v>
@@ -27821,7 +27821,7 @@
         <v>9</v>
       </c>
       <c r="B1053" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1053" s="2">
         <v>2004</v>
@@ -27847,7 +27847,7 @@
         <v>9</v>
       </c>
       <c r="B1054" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1054" s="2">
         <v>2005</v>
@@ -27873,7 +27873,7 @@
         <v>9</v>
       </c>
       <c r="B1055" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1055" s="2">
         <v>2006</v>
@@ -27899,7 +27899,7 @@
         <v>9</v>
       </c>
       <c r="B1056" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1056" s="2">
         <v>2007</v>
@@ -27925,7 +27925,7 @@
         <v>9</v>
       </c>
       <c r="B1057" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1057" s="2">
         <v>2008</v>
@@ -27951,7 +27951,7 @@
         <v>9</v>
       </c>
       <c r="B1058" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1058" s="2">
         <v>2009</v>
@@ -27977,7 +27977,7 @@
         <v>9</v>
       </c>
       <c r="B1059" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1059" s="2">
         <v>2010</v>
@@ -28003,7 +28003,7 @@
         <v>9</v>
       </c>
       <c r="B1060" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1060" s="2">
         <v>2011</v>
@@ -28029,7 +28029,7 @@
         <v>9</v>
       </c>
       <c r="B1061" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1061" s="2">
         <v>2012</v>
@@ -28055,7 +28055,7 @@
         <v>9</v>
       </c>
       <c r="B1062" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1062" s="2">
         <v>2013</v>
@@ -28081,7 +28081,7 @@
         <v>9</v>
       </c>
       <c r="B1063" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1063" s="2">
         <v>2014</v>
@@ -28107,7 +28107,7 @@
         <v>9</v>
       </c>
       <c r="B1064" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1064" s="2">
         <v>2015</v>
@@ -28133,7 +28133,7 @@
         <v>9</v>
       </c>
       <c r="B1065" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1065" s="2">
         <v>2016</v>
@@ -28159,7 +28159,7 @@
         <v>9</v>
       </c>
       <c r="B1066" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1066" s="2">
         <v>2017</v>
@@ -28185,7 +28185,7 @@
         <v>9</v>
       </c>
       <c r="B1067" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1067" s="2">
         <v>2018</v>
@@ -28211,7 +28211,7 @@
         <v>9</v>
       </c>
       <c r="B1068" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1068" s="2">
         <v>2019</v>
@@ -28237,7 +28237,7 @@
         <v>9</v>
       </c>
       <c r="B1069" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1069" s="2">
         <v>2020</v>
@@ -28263,7 +28263,7 @@
         <v>9</v>
       </c>
       <c r="B1070" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1070" s="2">
         <v>2021</v>
@@ -28289,7 +28289,7 @@
         <v>9</v>
       </c>
       <c r="B1071" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1071" s="2">
         <v>2022</v>
@@ -28315,7 +28315,7 @@
         <v>9</v>
       </c>
       <c r="B1072" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1072" s="2">
         <v>2023</v>
@@ -28341,7 +28341,7 @@
         <v>9</v>
       </c>
       <c r="B1073" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1073" s="2">
         <v>1961</v>
@@ -28367,7 +28367,7 @@
         <v>9</v>
       </c>
       <c r="B1074" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1074" s="2">
         <v>1962</v>
@@ -28393,7 +28393,7 @@
         <v>9</v>
       </c>
       <c r="B1075" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1075" s="2">
         <v>1963</v>
@@ -28419,7 +28419,7 @@
         <v>9</v>
       </c>
       <c r="B1076" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1076" s="2">
         <v>1964</v>
@@ -28445,7 +28445,7 @@
         <v>9</v>
       </c>
       <c r="B1077" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1077" s="2">
         <v>1965</v>
@@ -28471,7 +28471,7 @@
         <v>9</v>
       </c>
       <c r="B1078" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1078" s="2">
         <v>1966</v>
@@ -28497,7 +28497,7 @@
         <v>9</v>
       </c>
       <c r="B1079" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1079" s="2">
         <v>1967</v>
@@ -28523,7 +28523,7 @@
         <v>9</v>
       </c>
       <c r="B1080" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1080" s="2">
         <v>1968</v>
@@ -28549,7 +28549,7 @@
         <v>9</v>
       </c>
       <c r="B1081" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1081" s="2">
         <v>1969</v>
@@ -28575,7 +28575,7 @@
         <v>9</v>
       </c>
       <c r="B1082" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1082" s="2">
         <v>1970</v>
@@ -28601,7 +28601,7 @@
         <v>9</v>
       </c>
       <c r="B1083" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1083" s="2">
         <v>1971</v>
@@ -28627,7 +28627,7 @@
         <v>9</v>
       </c>
       <c r="B1084" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1084" s="2">
         <v>1972</v>
@@ -28653,7 +28653,7 @@
         <v>9</v>
       </c>
       <c r="B1085" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1085" s="2">
         <v>1973</v>
@@ -28679,7 +28679,7 @@
         <v>9</v>
       </c>
       <c r="B1086" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1086" s="2">
         <v>1974</v>
@@ -28705,7 +28705,7 @@
         <v>9</v>
       </c>
       <c r="B1087" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1087" s="2">
         <v>1975</v>
@@ -28731,7 +28731,7 @@
         <v>9</v>
       </c>
       <c r="B1088" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1088" s="2">
         <v>1976</v>
@@ -28757,7 +28757,7 @@
         <v>9</v>
       </c>
       <c r="B1089" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1089" s="2">
         <v>1977</v>
@@ -28783,7 +28783,7 @@
         <v>9</v>
       </c>
       <c r="B1090" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1090" s="2">
         <v>1978</v>
@@ -28809,7 +28809,7 @@
         <v>9</v>
       </c>
       <c r="B1091" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1091" s="2">
         <v>1979</v>
@@ -28835,7 +28835,7 @@
         <v>9</v>
       </c>
       <c r="B1092" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1092" s="2">
         <v>1980</v>
@@ -28861,7 +28861,7 @@
         <v>9</v>
       </c>
       <c r="B1093" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1093" s="2">
         <v>1981</v>
@@ -28887,7 +28887,7 @@
         <v>9</v>
       </c>
       <c r="B1094" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1094" s="2">
         <v>1982</v>
@@ -28913,7 +28913,7 @@
         <v>9</v>
       </c>
       <c r="B1095" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1095" s="2">
         <v>1983</v>
@@ -28939,7 +28939,7 @@
         <v>9</v>
       </c>
       <c r="B1096" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1096" s="2">
         <v>1984</v>
@@ -28965,7 +28965,7 @@
         <v>9</v>
       </c>
       <c r="B1097" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1097" s="2">
         <v>1985</v>
@@ -28991,7 +28991,7 @@
         <v>9</v>
       </c>
       <c r="B1098" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1098" s="2">
         <v>1986</v>
@@ -29017,7 +29017,7 @@
         <v>9</v>
       </c>
       <c r="B1099" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1099" s="2">
         <v>1987</v>
@@ -29043,7 +29043,7 @@
         <v>9</v>
       </c>
       <c r="B1100" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1100" s="2">
         <v>1988</v>
@@ -29069,7 +29069,7 @@
         <v>9</v>
       </c>
       <c r="B1101" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1101" s="2">
         <v>1989</v>
@@ -29095,7 +29095,7 @@
         <v>9</v>
       </c>
       <c r="B1102" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1102" s="2">
         <v>1990</v>
@@ -29121,7 +29121,7 @@
         <v>9</v>
       </c>
       <c r="B1103" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1103" s="2">
         <v>1991</v>
@@ -29147,7 +29147,7 @@
         <v>9</v>
       </c>
       <c r="B1104" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1104" s="2">
         <v>1992</v>
@@ -29173,7 +29173,7 @@
         <v>9</v>
       </c>
       <c r="B1105" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1105" s="2">
         <v>1993</v>
@@ -29199,7 +29199,7 @@
         <v>9</v>
       </c>
       <c r="B1106" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1106" s="2">
         <v>1994</v>
@@ -29225,7 +29225,7 @@
         <v>9</v>
       </c>
       <c r="B1107" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1107" s="2">
         <v>1995</v>
@@ -29251,7 +29251,7 @@
         <v>9</v>
       </c>
       <c r="B1108" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1108" s="2">
         <v>1996</v>
@@ -29277,7 +29277,7 @@
         <v>9</v>
       </c>
       <c r="B1109" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1109" s="2">
         <v>1997</v>
@@ -29303,7 +29303,7 @@
         <v>9</v>
       </c>
       <c r="B1110" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1110" s="2">
         <v>1998</v>
@@ -29329,7 +29329,7 @@
         <v>9</v>
       </c>
       <c r="B1111" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1111" s="2">
         <v>1999</v>
@@ -29355,7 +29355,7 @@
         <v>9</v>
       </c>
       <c r="B1112" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1112" s="2">
         <v>2000</v>
@@ -29381,7 +29381,7 @@
         <v>9</v>
       </c>
       <c r="B1113" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1113" s="2">
         <v>2001</v>
@@ -29407,7 +29407,7 @@
         <v>9</v>
       </c>
       <c r="B1114" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1114" s="2">
         <v>2002</v>
@@ -29433,7 +29433,7 @@
         <v>9</v>
       </c>
       <c r="B1115" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1115" s="2">
         <v>2003</v>
@@ -29459,7 +29459,7 @@
         <v>9</v>
       </c>
       <c r="B1116" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1116" s="2">
         <v>2004</v>
@@ -29485,7 +29485,7 @@
         <v>9</v>
       </c>
       <c r="B1117" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1117" s="2">
         <v>2005</v>
@@ -29511,7 +29511,7 @@
         <v>9</v>
       </c>
       <c r="B1118" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1118" s="2">
         <v>2006</v>
@@ -29537,7 +29537,7 @@
         <v>9</v>
       </c>
       <c r="B1119" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1119" s="2">
         <v>2007</v>
@@ -29563,7 +29563,7 @@
         <v>9</v>
       </c>
       <c r="B1120" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1120" s="2">
         <v>2008</v>
@@ -29589,7 +29589,7 @@
         <v>9</v>
       </c>
       <c r="B1121" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1121" s="2">
         <v>2009</v>
@@ -29615,7 +29615,7 @@
         <v>9</v>
       </c>
       <c r="B1122" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1122" s="2">
         <v>2010</v>
@@ -29641,7 +29641,7 @@
         <v>9</v>
       </c>
       <c r="B1123" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1123" s="2">
         <v>2011</v>
@@ -29667,7 +29667,7 @@
         <v>9</v>
       </c>
       <c r="B1124" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1124" s="2">
         <v>2012</v>
@@ -29693,7 +29693,7 @@
         <v>9</v>
       </c>
       <c r="B1125" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1125" s="2">
         <v>2013</v>
@@ -29719,7 +29719,7 @@
         <v>9</v>
       </c>
       <c r="B1126" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1126" s="2">
         <v>2014</v>
@@ -29745,7 +29745,7 @@
         <v>9</v>
       </c>
       <c r="B1127" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1127" s="2">
         <v>2015</v>
@@ -29771,7 +29771,7 @@
         <v>9</v>
       </c>
       <c r="B1128" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1128" s="2">
         <v>2016</v>
@@ -29797,7 +29797,7 @@
         <v>9</v>
       </c>
       <c r="B1129" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1129" s="2">
         <v>2017</v>
@@ -29823,7 +29823,7 @@
         <v>9</v>
       </c>
       <c r="B1130" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1130" s="2">
         <v>2018</v>
@@ -29849,7 +29849,7 @@
         <v>9</v>
       </c>
       <c r="B1131" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1131" s="2">
         <v>2019</v>
@@ -29875,7 +29875,7 @@
         <v>9</v>
       </c>
       <c r="B1132" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1132" s="2">
         <v>2020</v>
@@ -29901,7 +29901,7 @@
         <v>9</v>
       </c>
       <c r="B1133" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1133" s="2">
         <v>2021</v>
@@ -29927,7 +29927,7 @@
         <v>9</v>
       </c>
       <c r="B1134" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1134" s="2">
         <v>2022</v>
@@ -29953,7 +29953,7 @@
         <v>9</v>
       </c>
       <c r="B1135" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1135" s="2">
         <v>2023</v>

</xml_diff>